<commit_message>
add movie exeption fixed
</commit_message>
<xml_diff>
--- a/Main_assignment/MovieData.xlsx
+++ b/Main_assignment/MovieData.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -608,6 +608,38 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>gadar</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ACtion</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>sunny deol</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>